<commit_message>
revise portfolio return to excessive return
</commit_message>
<xml_diff>
--- a/result/Final_Portfolio_Stats.xlsx
+++ b/result/Final_Portfolio_Stats.xlsx
@@ -538,19 +538,19 @@
         <v>0.4221851803620262</v>
       </c>
       <c r="L2" t="n">
-        <v>1.573613052034996</v>
+        <v>1.573611225101008</v>
       </c>
       <c r="M2" t="n">
         <v>0.1200055342634963</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9197820533866884</v>
+        <v>0.9197767556461826</v>
       </c>
       <c r="O2" t="n">
-        <v>5.438849319567214e-05</v>
+        <v>3.840663667156422e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01379987887226197</v>
+        <v>0.009725272662092665</v>
       </c>
     </row>
     <row r="3">

</xml_diff>